<commit_message>
Second alt. This is the key solution
</commit_message>
<xml_diff>
--- a/CH-168 Custom Grouping.xlsx
+++ b/CH-168 Custom Grouping.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66F336F4-FE17-48FB-9D97-DCA976020C65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9FC64B5-155C-41E4-96D9-EEC338A4091B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
     <sheet name="Alt1" sheetId="3" r:id="rId3"/>
+    <sheet name="Alt2" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Alt1'!$B$2:$D$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Alt2'!$B$2:$D$26</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$B$2:$D$26</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$2:$D$26</definedName>
   </definedNames>
@@ -65,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="12">
   <si>
     <t>Question</t>
   </si>
@@ -86,6 +88,21 @@
   </si>
   <si>
     <t>Very nice use of expanding range</t>
+  </si>
+  <si>
+    <t>This is very clever.</t>
+  </si>
+  <si>
+    <t>I like the use of SCAN with an eta MIN</t>
+  </si>
+  <si>
+    <t>The XMATCH is clever. Let's play with that a  bit.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basically, he does nothing with the </t>
+  </si>
+  <si>
+    <t>data after the comparisons are done.</t>
   </si>
 </sst>
 </file>
@@ -2941,8 +2958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{143CD192-E5DB-4B76-9529-332B32AF32D1}">
   <dimension ref="A1:N53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView topLeftCell="A17" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3631,4 +3648,1016 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9B5A437-44C9-47FE-B1A1-E29D886609F8}">
+  <dimension ref="A1:N52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.109375" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.21875" customWidth="1"/>
+    <col min="6" max="6" width="23.6640625" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="32"/>
+      <c r="E1"/>
+      <c r="G1" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+    </row>
+    <row r="2" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2"/>
+      <c r="G2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="18">
+        <v>45292</v>
+      </c>
+      <c r="C3" s="19">
+        <v>47</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3"/>
+      <c r="G3" s="18">
+        <v>45292</v>
+      </c>
+      <c r="H3" s="25">
+        <v>47</v>
+      </c>
+      <c r="I3" s="25">
+        <v>1</v>
+      </c>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="9"/>
+    </row>
+    <row r="4" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="18">
+        <v>45293</v>
+      </c>
+      <c r="C4" s="19">
+        <v>62</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4"/>
+      <c r="G4" s="18">
+        <v>45293</v>
+      </c>
+      <c r="H4" s="25">
+        <v>62</v>
+      </c>
+      <c r="I4" s="25">
+        <v>1</v>
+      </c>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="9"/>
+    </row>
+    <row r="5" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="18">
+        <v>45294</v>
+      </c>
+      <c r="C5" s="19">
+        <v>99</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5"/>
+      <c r="G5" s="18">
+        <v>45294</v>
+      </c>
+      <c r="H5" s="25">
+        <v>99</v>
+      </c>
+      <c r="I5" s="25">
+        <v>1</v>
+      </c>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="9"/>
+    </row>
+    <row r="6" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="12">
+        <v>45295</v>
+      </c>
+      <c r="C6" s="13">
+        <v>43</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6"/>
+      <c r="G6" s="12">
+        <v>45295</v>
+      </c>
+      <c r="H6" s="26">
+        <v>43</v>
+      </c>
+      <c r="I6" s="26">
+        <v>2</v>
+      </c>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="9"/>
+    </row>
+    <row r="7" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="12">
+        <v>45296</v>
+      </c>
+      <c r="C7" s="13">
+        <v>55</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7"/>
+      <c r="G7" s="12">
+        <v>45296</v>
+      </c>
+      <c r="H7" s="26">
+        <v>55</v>
+      </c>
+      <c r="I7" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="12">
+        <v>45297</v>
+      </c>
+      <c r="C8" s="13">
+        <v>65</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8"/>
+      <c r="G8" s="12">
+        <v>45297</v>
+      </c>
+      <c r="H8" s="26">
+        <v>65</v>
+      </c>
+      <c r="I8" s="26">
+        <v>2</v>
+      </c>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="L8"/>
+      <c r="M8"/>
+    </row>
+    <row r="9" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="12">
+        <v>45298</v>
+      </c>
+      <c r="C9" s="13">
+        <v>72</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9"/>
+      <c r="G9" s="12">
+        <v>45298</v>
+      </c>
+      <c r="H9" s="26">
+        <v>72</v>
+      </c>
+      <c r="I9" s="26">
+        <v>2</v>
+      </c>
+      <c r="J9"/>
+      <c r="K9"/>
+      <c r="L9"/>
+      <c r="M9"/>
+    </row>
+    <row r="10" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="12">
+        <v>45299</v>
+      </c>
+      <c r="C10" s="13">
+        <v>110</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10"/>
+      <c r="G10" s="12">
+        <v>45299</v>
+      </c>
+      <c r="H10" s="26">
+        <v>110</v>
+      </c>
+      <c r="I10" s="26">
+        <v>2</v>
+      </c>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="M10"/>
+    </row>
+    <row r="11" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="12">
+        <v>45300</v>
+      </c>
+      <c r="C11" s="13">
+        <v>106</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11"/>
+      <c r="G11" s="12">
+        <v>45300</v>
+      </c>
+      <c r="H11" s="26">
+        <v>106</v>
+      </c>
+      <c r="I11" s="26">
+        <v>2</v>
+      </c>
+      <c r="J11"/>
+      <c r="K11"/>
+      <c r="L11"/>
+      <c r="M11"/>
+    </row>
+    <row r="12" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="20">
+        <v>45301</v>
+      </c>
+      <c r="C12" s="21">
+        <v>30</v>
+      </c>
+      <c r="D12" s="9"/>
+      <c r="E12" s="10"/>
+      <c r="F12"/>
+      <c r="G12" s="20">
+        <v>45301</v>
+      </c>
+      <c r="H12" s="27">
+        <v>30</v>
+      </c>
+      <c r="I12" s="27">
+        <v>3</v>
+      </c>
+      <c r="J12"/>
+      <c r="K12"/>
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B13" s="20">
+        <v>45302</v>
+      </c>
+      <c r="C13" s="21">
+        <v>103</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="E13" s="10"/>
+      <c r="G13" s="20">
+        <v>45302</v>
+      </c>
+      <c r="H13" s="27">
+        <v>103</v>
+      </c>
+      <c r="I13" s="27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B14" s="20">
+        <v>45303</v>
+      </c>
+      <c r="C14" s="21">
+        <v>100</v>
+      </c>
+      <c r="D14" s="9"/>
+      <c r="E14" s="10"/>
+      <c r="G14" s="20">
+        <v>45303</v>
+      </c>
+      <c r="H14" s="27">
+        <v>100</v>
+      </c>
+      <c r="I14" s="27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="20">
+        <v>45304</v>
+      </c>
+      <c r="C15" s="21">
+        <v>85</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="10"/>
+      <c r="G15" s="20">
+        <v>45304</v>
+      </c>
+      <c r="H15" s="27">
+        <v>85</v>
+      </c>
+      <c r="I15" s="27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="20">
+        <v>45305</v>
+      </c>
+      <c r="C16" s="21">
+        <v>90</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="10"/>
+      <c r="G16" s="20">
+        <v>45305</v>
+      </c>
+      <c r="H16" s="27">
+        <v>90</v>
+      </c>
+      <c r="I16" s="27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="20">
+        <v>45306</v>
+      </c>
+      <c r="C17" s="21">
+        <v>80</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="10"/>
+      <c r="G17" s="20">
+        <v>45306</v>
+      </c>
+      <c r="H17" s="27">
+        <v>80</v>
+      </c>
+      <c r="I17" s="27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="20">
+        <v>45307</v>
+      </c>
+      <c r="C18" s="21">
+        <v>61</v>
+      </c>
+      <c r="D18" s="9"/>
+      <c r="E18" s="10"/>
+      <c r="G18" s="20">
+        <v>45307</v>
+      </c>
+      <c r="H18" s="27">
+        <v>61</v>
+      </c>
+      <c r="I18" s="27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="22">
+        <v>45308</v>
+      </c>
+      <c r="C19" s="23">
+        <v>25</v>
+      </c>
+      <c r="D19" s="9"/>
+      <c r="E19" s="10"/>
+      <c r="G19" s="22">
+        <v>45308</v>
+      </c>
+      <c r="H19" s="28">
+        <v>25</v>
+      </c>
+      <c r="I19" s="28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="22">
+        <v>45309</v>
+      </c>
+      <c r="C20" s="23">
+        <v>55</v>
+      </c>
+      <c r="D20" s="9"/>
+      <c r="E20" s="1"/>
+      <c r="G20" s="22">
+        <v>45309</v>
+      </c>
+      <c r="H20" s="28">
+        <v>55</v>
+      </c>
+      <c r="I20" s="28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="22">
+        <v>45310</v>
+      </c>
+      <c r="C21" s="23">
+        <v>52</v>
+      </c>
+      <c r="D21" s="9"/>
+      <c r="E21" s="1"/>
+      <c r="G21" s="22">
+        <v>45310</v>
+      </c>
+      <c r="H21" s="28">
+        <v>52</v>
+      </c>
+      <c r="I21" s="28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="22">
+        <v>45311</v>
+      </c>
+      <c r="C22" s="23">
+        <v>75</v>
+      </c>
+      <c r="D22" s="9"/>
+      <c r="E22" s="1"/>
+      <c r="G22" s="22">
+        <v>45311</v>
+      </c>
+      <c r="H22" s="28">
+        <v>75</v>
+      </c>
+      <c r="I22" s="28">
+        <v>4</v>
+      </c>
+      <c r="N22" s="2"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+      <c r="B23" s="22">
+        <v>45312</v>
+      </c>
+      <c r="C23" s="23">
+        <v>84</v>
+      </c>
+      <c r="D23" s="9"/>
+      <c r="E23" s="1"/>
+      <c r="G23" s="22">
+        <v>45312</v>
+      </c>
+      <c r="H23" s="28">
+        <v>84</v>
+      </c>
+      <c r="I23" s="28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B24" s="22">
+        <v>45313</v>
+      </c>
+      <c r="C24" s="23">
+        <v>94</v>
+      </c>
+      <c r="D24" s="9"/>
+      <c r="E24" s="1"/>
+      <c r="G24" s="22">
+        <v>45313</v>
+      </c>
+      <c r="H24" s="28">
+        <v>94</v>
+      </c>
+      <c r="I24" s="28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B25" s="14">
+        <v>45314</v>
+      </c>
+      <c r="C25" s="15">
+        <v>18</v>
+      </c>
+      <c r="D25" s="9"/>
+      <c r="E25" s="1"/>
+      <c r="G25" s="14">
+        <v>45314</v>
+      </c>
+      <c r="H25" s="29">
+        <v>18</v>
+      </c>
+      <c r="I25" s="29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B26" s="16">
+        <v>45315</v>
+      </c>
+      <c r="C26" s="17">
+        <v>105</v>
+      </c>
+      <c r="D26" s="9"/>
+      <c r="G26" s="16">
+        <v>45315</v>
+      </c>
+      <c r="H26" s="30">
+        <v>105</v>
+      </c>
+      <c r="I26" s="30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B29" s="4" cm="1">
+        <f t="array" ref="B29:D52">_xlfn.LET(_xlpm.s,_xlfn.SCAN(,C3:C26,_xleta.MIN),_xlfn.HSTACK(B3:C26,_xlfn.XMATCH(_xlpm.s,_xlfn.UNIQUE(_xlpm.s))))</f>
+        <v>45292</v>
+      </c>
+      <c r="C29">
+        <v>47</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="F29" t="s">
+        <v>7</v>
+      </c>
+      <c r="I29" cm="1">
+        <f t="array" ref="I29:I52">_xlfn.SCAN(,C3:C26,_xleta.MIN)</f>
+        <v>47</v>
+      </c>
+      <c r="J29" cm="1">
+        <f t="array" ref="J29:J33">_xlfn.UNIQUE(_xlfn.ANCHORARRAY(I29))</f>
+        <v>47</v>
+      </c>
+      <c r="K29" cm="1">
+        <f t="array" ref="K29:K52">_xlfn.XMATCH(_xlfn.ANCHORARRAY(I29),_xlfn.ANCHORARRAY(J29))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B30" s="4">
+        <v>45293</v>
+      </c>
+      <c r="C30">
+        <v>62</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="F30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I30">
+        <v>47</v>
+      </c>
+      <c r="J30">
+        <v>43</v>
+      </c>
+      <c r="K30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B31" s="4">
+        <v>45294</v>
+      </c>
+      <c r="C31">
+        <v>99</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="F31" t="s">
+        <v>9</v>
+      </c>
+      <c r="I31">
+        <v>47</v>
+      </c>
+      <c r="J31">
+        <v>30</v>
+      </c>
+      <c r="K31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B32" s="4">
+        <v>45295</v>
+      </c>
+      <c r="C32">
+        <v>43</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+      <c r="F32" t="s">
+        <v>10</v>
+      </c>
+      <c r="I32">
+        <v>43</v>
+      </c>
+      <c r="J32">
+        <v>25</v>
+      </c>
+      <c r="K32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B33" s="4">
+        <v>45296</v>
+      </c>
+      <c r="C33">
+        <v>55</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+      <c r="F33" t="s">
+        <v>11</v>
+      </c>
+      <c r="I33">
+        <v>43</v>
+      </c>
+      <c r="J33">
+        <v>18</v>
+      </c>
+      <c r="K33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B34" s="4">
+        <v>45297</v>
+      </c>
+      <c r="C34">
+        <v>65</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="I34">
+        <v>43</v>
+      </c>
+      <c r="K34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B35" s="4">
+        <v>45298</v>
+      </c>
+      <c r="C35">
+        <v>72</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
+      </c>
+      <c r="I35">
+        <v>43</v>
+      </c>
+      <c r="K35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B36" s="4">
+        <v>45299</v>
+      </c>
+      <c r="C36">
+        <v>110</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+      <c r="I36">
+        <v>43</v>
+      </c>
+      <c r="K36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B37" s="4">
+        <v>45300</v>
+      </c>
+      <c r="C37">
+        <v>106</v>
+      </c>
+      <c r="D37">
+        <v>2</v>
+      </c>
+      <c r="I37">
+        <v>43</v>
+      </c>
+      <c r="K37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B38" s="4">
+        <v>45301</v>
+      </c>
+      <c r="C38">
+        <v>30</v>
+      </c>
+      <c r="D38">
+        <v>3</v>
+      </c>
+      <c r="I38">
+        <v>30</v>
+      </c>
+      <c r="K38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B39" s="4">
+        <v>45302</v>
+      </c>
+      <c r="C39">
+        <v>103</v>
+      </c>
+      <c r="D39">
+        <v>3</v>
+      </c>
+      <c r="I39">
+        <v>30</v>
+      </c>
+      <c r="K39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B40" s="4">
+        <v>45303</v>
+      </c>
+      <c r="C40">
+        <v>100</v>
+      </c>
+      <c r="D40">
+        <v>3</v>
+      </c>
+      <c r="I40">
+        <v>30</v>
+      </c>
+      <c r="K40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B41" s="4">
+        <v>45304</v>
+      </c>
+      <c r="C41">
+        <v>85</v>
+      </c>
+      <c r="D41">
+        <v>3</v>
+      </c>
+      <c r="I41">
+        <v>30</v>
+      </c>
+      <c r="K41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B42" s="4">
+        <v>45305</v>
+      </c>
+      <c r="C42">
+        <v>90</v>
+      </c>
+      <c r="D42">
+        <v>3</v>
+      </c>
+      <c r="I42">
+        <v>30</v>
+      </c>
+      <c r="K42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B43" s="4">
+        <v>45306</v>
+      </c>
+      <c r="C43">
+        <v>80</v>
+      </c>
+      <c r="D43">
+        <v>3</v>
+      </c>
+      <c r="I43">
+        <v>30</v>
+      </c>
+      <c r="K43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B44" s="4">
+        <v>45307</v>
+      </c>
+      <c r="C44">
+        <v>61</v>
+      </c>
+      <c r="D44">
+        <v>3</v>
+      </c>
+      <c r="I44">
+        <v>30</v>
+      </c>
+      <c r="K44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B45" s="4">
+        <v>45308</v>
+      </c>
+      <c r="C45">
+        <v>25</v>
+      </c>
+      <c r="D45">
+        <v>4</v>
+      </c>
+      <c r="I45">
+        <v>25</v>
+      </c>
+      <c r="K45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B46" s="4">
+        <v>45309</v>
+      </c>
+      <c r="C46">
+        <v>55</v>
+      </c>
+      <c r="D46">
+        <v>4</v>
+      </c>
+      <c r="I46">
+        <v>25</v>
+      </c>
+      <c r="K46">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B47" s="4">
+        <v>45310</v>
+      </c>
+      <c r="C47">
+        <v>52</v>
+      </c>
+      <c r="D47">
+        <v>4</v>
+      </c>
+      <c r="I47">
+        <v>25</v>
+      </c>
+      <c r="K47">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B48" s="4">
+        <v>45311</v>
+      </c>
+      <c r="C48">
+        <v>75</v>
+      </c>
+      <c r="D48">
+        <v>4</v>
+      </c>
+      <c r="I48">
+        <v>25</v>
+      </c>
+      <c r="K48">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B49" s="4">
+        <v>45312</v>
+      </c>
+      <c r="C49">
+        <v>84</v>
+      </c>
+      <c r="D49">
+        <v>4</v>
+      </c>
+      <c r="I49">
+        <v>25</v>
+      </c>
+      <c r="K49">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B50" s="4">
+        <v>45313</v>
+      </c>
+      <c r="C50">
+        <v>94</v>
+      </c>
+      <c r="D50">
+        <v>4</v>
+      </c>
+      <c r="I50">
+        <v>25</v>
+      </c>
+      <c r="K50">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B51" s="4">
+        <v>45314</v>
+      </c>
+      <c r="C51">
+        <v>18</v>
+      </c>
+      <c r="D51">
+        <v>5</v>
+      </c>
+      <c r="I51">
+        <v>18</v>
+      </c>
+      <c r="K51">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B52" s="4">
+        <v>45315</v>
+      </c>
+      <c r="C52">
+        <v>105</v>
+      </c>
+      <c r="D52">
+        <v>5</v>
+      </c>
+      <c r="I52">
+        <v>18</v>
+      </c>
+      <c r="K52">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="G1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>